<commit_message>
Added link for ADS
</commit_message>
<xml_diff>
--- a/input BOM.xlsx
+++ b/input BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Description</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Can be anything from 20k to 50k</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/general-purpose-adcs/7094550/</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -137,6 +140,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,7 +459,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +530,9 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C5">
         <v>2</v>
       </c>
@@ -572,8 +578,9 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B7" r:id="rId4"/>
     <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New gerber files. Added labels in the BOM
</commit_message>
<xml_diff>
--- a/input BOM.xlsx
+++ b/input BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -48,18 +48,9 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791569/</t>
   </si>
   <si>
-    <t>ADC (ADS1015IDGSR)</t>
-  </si>
-  <si>
     <t>AD623ARZ-R7</t>
   </si>
   <si>
-    <t>2 pin female header</t>
-  </si>
-  <si>
-    <t>http://china.rs-online.com/web/p/pcb-sockets/8277725/</t>
-  </si>
-  <si>
     <t>30k surface mount resistors 0805</t>
   </si>
   <si>
@@ -82,6 +73,30 @@
   </si>
   <si>
     <t>http://china.rs-online.com/web/p/general-purpose-adcs/7094550/</t>
+  </si>
+  <si>
+    <t>Place Labels</t>
+  </si>
+  <si>
+    <t>C1, C2, ADC1Cap, ADC2Cap, Cref, Csr, C3, C4, C5, C6, C7, C8, ADCap1, ADCap2, OpCap</t>
+  </si>
+  <si>
+    <t>Rr1, R2, Rr2</t>
+  </si>
+  <si>
+    <t>R1,R3, R4, R5, R7, R6, R8, R9,R10,R11, R12, R13</t>
+  </si>
+  <si>
+    <t>ADS1015IDGSR</t>
+  </si>
+  <si>
+    <t>ADS1015-1, ADS1015-2</t>
+  </si>
+  <si>
+    <t>AD623-1, AD623-2</t>
+  </si>
+  <si>
+    <t>Rsr1, Rsr2</t>
   </si>
 </sst>
 </file>
@@ -456,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +482,11 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="52.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,10 +497,13 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -495,10 +514,13 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -509,10 +531,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -523,52 +548,53 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -577,10 +603,9 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed some components in the input BOM
</commit_message>
<xml_diff>
--- a/input BOM.xlsx
+++ b/input BOM.xlsx
@@ -30,15 +30,9 @@
     <t>3.2uF surface mount capacitors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/6911161/</t>
-  </si>
-  <si>
     <t>10k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6789667/</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>30k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -97,6 +88,15 @@
   </si>
   <si>
     <t>Rsr1, Rsr2</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791263/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230562/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/7236054/</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,118 +494,115 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added to BOM, is now complete
</commit_message>
<xml_diff>
--- a/input BOM.xlsx
+++ b/input BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -97,6 +97,33 @@
   </si>
   <si>
     <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/7236054/</t>
+  </si>
+  <si>
+    <t>10 pin female header</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/pcb-sockets/7655745/</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>2 pin male header</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com//web/p/pcb-headers/2518086/</t>
+  </si>
+  <si>
+    <t>J3, J4</t>
+  </si>
+  <si>
+    <t>dual opamp, TL072CD</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/operational-amplifiers/0857907/</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
 </sst>
 </file>
@@ -471,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +509,7 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="52.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="4" width="76.5703125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -597,12 +624,55 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3" display="http://china.rs-online.com/web/p/pcb-headers/2518086/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>